<commit_message>
start miller rabin primality test code
</commit_message>
<xml_diff>
--- a/5. RSA Assignment 2 - Graphing/Graphs.xlsx
+++ b/5. RSA Assignment 2 - Graphing/Graphs.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -705,11 +705,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2041184912"/>
-        <c:axId val="2042664080"/>
+        <c:axId val="-159706592"/>
+        <c:axId val="-159704272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2041184912"/>
+        <c:axId val="-159706592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -752,7 +752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2042664080"/>
+        <c:crossAx val="-159704272"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -761,7 +761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2042664080"/>
+        <c:axId val="-159704272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1500.0"/>
@@ -813,7 +813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2041184912"/>
+        <c:crossAx val="-159706592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1265,11 +1265,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1970192624"/>
-        <c:axId val="1970194400"/>
+        <c:axId val="-159677856"/>
+        <c:axId val="-159675536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1970192624"/>
+        <c:axId val="-159677856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1312,7 +1312,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1970194400"/>
+        <c:crossAx val="-159675536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1320,7 +1320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1970194400"/>
+        <c:axId val="-159675536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1370,7 +1370,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1970192624"/>
+        <c:crossAx val="-159677856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1785,11 +1785,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2038577632"/>
-        <c:axId val="2045351952"/>
+        <c:axId val="-159655344"/>
+        <c:axId val="-159653024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2038577632"/>
+        <c:axId val="-159655344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1832,7 +1832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2045351952"/>
+        <c:crossAx val="-159653024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1840,7 +1840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2045351952"/>
+        <c:axId val="-159653024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1890,7 +1890,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2038577632"/>
+        <c:crossAx val="-159655344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4192,7 +4192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I6" workbookViewId="0">
       <selection activeCell="AA35" sqref="AA35"/>
     </sheetView>
   </sheetViews>

</xml_diff>